<commit_message>
Corrected the swapped cal coefficients for speed and controller current
</commit_message>
<xml_diff>
--- a/Executable/Files/Template.xlsx
+++ b/Executable/Files/Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
   <si>
     <t>Serial Numbers</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>(Celsius)</t>
+  </si>
+  <si>
+    <t>Desired Parameters</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,23 +340,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,25 +392,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,7 +703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -720,164 +711,192 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" customWidth="1"/>
-    <col min="14" max="15" width="13.7109375" customWidth="1"/>
+    <col min="1" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
+    <col min="13" max="14" width="26.7109375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
       <c r="M1" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A2" s="22" t="s">
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="26" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="33"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A3" s="22" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="26" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="33"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="18"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="15"/>
       <c r="M5" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="13" t="s">
+      <c r="N5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B6" s="11"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="29"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -917,8 +936,11 @@
       <c r="M9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+      <c r="N9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -956,6 +978,9 @@
         <v>21</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -979,7 +1004,6 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C6:M7"/>
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="A4:B4"/>
@@ -993,6 +1017,7 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C6:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1001,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -1009,230 +1034,261 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" customWidth="1"/>
-    <col min="14" max="15" width="13.7109375" customWidth="1"/>
+    <col min="1" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
+    <col min="13" max="14" width="26.7109375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A2" s="22" t="s">
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="26" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="33"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A3" s="22" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="26" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="33"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="18"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="15"/>
       <c r="M5" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="13" t="s">
+      <c r="N5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A9" s="4" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="29"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+      <c r="N9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="5" t="s">
@@ -1245,6 +1301,9 @@
         <v>21</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1262,6 +1321,8 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C6:N7"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
@@ -1275,13 +1336,11 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:M7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1298,9 +1357,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="9" width="13.7109375" customWidth="1"/>
+    <col min="3" max="9" width="13.7109375" style="9" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="12" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>